<commit_message>
added another second level page
</commit_message>
<xml_diff>
--- a/Lab/doc/PriceList.xlsx
+++ b/Lab/doc/PriceList.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -44,42 +44,6 @@
   </si>
   <si>
     <t>Price, $</t>
-  </si>
-  <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
-    <t>0004</t>
-  </si>
-  <si>
-    <t>0005</t>
-  </si>
-  <si>
-    <t>0006</t>
-  </si>
-  <si>
-    <t>0007</t>
-  </si>
-  <si>
-    <t>0008</t>
-  </si>
-  <si>
-    <t>0009</t>
-  </si>
-  <si>
-    <t>0010</t>
-  </si>
-  <si>
-    <t>0011</t>
-  </si>
-  <si>
-    <t>0012</t>
   </si>
   <si>
     <t>LAMBORGHINI SIAN</t>
@@ -565,14 +529,14 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.88671875" style="6" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="10" customWidth="1"/>
     <col min="4" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
@@ -588,135 +552,135 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="12">
-        <v>100000</v>
+        <v>3600000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" s="12">
-        <v>100000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" s="12">
-        <v>100000</v>
+        <v>270000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="12">
-        <v>100000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="C6" s="12">
-        <v>100000</v>
+        <v>2700000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="C7" s="12">
-        <v>100000</v>
+        <v>5800000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="12">
-        <v>100000</v>
+        <v>320000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="12">
-        <v>100000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="C10" s="12">
-        <v>100000</v>
+        <v>205000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="C11" s="12">
-        <v>100000</v>
+        <v>95000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" s="12">
-        <v>100000</v>
+        <v>280000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="12">
-        <v>100000</v>
+        <v>710000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -774,9 +738,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A4 A5:A13" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>